<commit_message>
add telaah obat EMR OBAT
</commit_message>
<xml_diff>
--- a/SI_Apotek_Pelayanan/bin/Debug/Report/LaporanStokOpnameXLSIO.xlsx
+++ b/SI_Apotek_Pelayanan/bin/Debug/Report/LaporanStokOpnameXLSIO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="9390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="9390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="stokOpname" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
   <si>
     <t>PEMERINTAH KABUPATEN PEKALONGAN</t>
   </si>
@@ -89,9 +89,6 @@
     <t>KOREKSI KELUAR</t>
   </si>
   <si>
-    <t>%Data.nmbarang;insert:copystyles</t>
-  </si>
-  <si>
     <t>%Data.stokawal</t>
   </si>
   <si>
@@ -204,13 +201,46 @@
   </si>
   <si>
     <t>RETUR OBT RWT INAP</t>
+  </si>
+  <si>
+    <t>KODE BARANG</t>
+  </si>
+  <si>
+    <t>KODE AKUN 108</t>
+  </si>
+  <si>
+    <t>%Data.kode_akun108</t>
+  </si>
+  <si>
+    <t>%Data.nmbarang</t>
+  </si>
+  <si>
+    <t>%Data.noUrut</t>
+  </si>
+  <si>
+    <t>%Data.kdbarang;insert:copystyles</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> SISA </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>STOK</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +260,19 @@
       <color theme="1"/>
       <name val="Tahoma"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -357,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -372,9 +415,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -391,12 +431,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -411,6 +473,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -717,27 +785,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" style="2" customWidth="1"/>
-    <col min="3" max="5" width="11" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="2" customWidth="1"/>
-    <col min="8" max="14" width="11" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="23.140625" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="23.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" style="2" customWidth="1"/>
+    <col min="5" max="7" width="11" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="2" customWidth="1"/>
+    <col min="10" max="16" width="11" style="2" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="23.140625" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -748,12 +818,14 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -764,12 +836,14 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -780,306 +854,382 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:19">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:19">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A10" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="C10" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="E10" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="F10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="21" t="s">
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="O10" s="17" t="s">
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q10" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="P10" s="19" t="s">
+      <c r="R10" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="Q10" s="19" t="s">
+      <c r="S10" s="26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="1" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="4" t="s">
+    <row r="11" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="H11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="K11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="M11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N11" s="20"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="P11" s="27"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="5">
         <v>1</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5">
         <v>2</v>
       </c>
-      <c r="C12" s="5">
+      <c r="E12" s="5">
         <v>3</v>
       </c>
-      <c r="D12" s="5">
+      <c r="F12" s="5">
         <v>4</v>
       </c>
-      <c r="E12" s="5">
+      <c r="G12" s="5">
         <v>5</v>
       </c>
-      <c r="F12" s="5">
+      <c r="H12" s="5">
         <v>6</v>
       </c>
-      <c r="G12" s="5">
+      <c r="I12" s="5">
         <v>7</v>
       </c>
-      <c r="H12" s="5">
+      <c r="J12" s="5">
         <v>8</v>
       </c>
-      <c r="I12" s="5">
+      <c r="K12" s="5">
         <v>9</v>
       </c>
-      <c r="J12" s="5">
+      <c r="L12" s="5">
         <v>10</v>
       </c>
-      <c r="K12" s="5">
+      <c r="M12" s="5">
         <v>11</v>
       </c>
-      <c r="L12" s="5">
+      <c r="N12" s="5">
         <v>12</v>
       </c>
-      <c r="M12" s="5">
+      <c r="O12" s="5">
         <v>13</v>
       </c>
-      <c r="N12" s="5">
+      <c r="P12" s="5">
         <v>14</v>
       </c>
-      <c r="O12" s="5">
+      <c r="Q12" s="5">
         <v>15</v>
       </c>
-      <c r="P12" s="5">
+      <c r="R12" s="5">
         <v>16</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="S12" s="5">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="6">
-        <v>1</v>
-      </c>
-      <c r="B13" s="7" t="s">
+    <row r="13" spans="1:19">
+      <c r="A13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="H13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="8" t="s">
+      <c r="J13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="K13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="L13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="M13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="N13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="O13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="P13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="Q13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="O13" s="6" t="s">
+      <c r="R13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="P13" s="8" t="s">
+      <c r="S13" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="Q13" s="8" t="s">
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q15" s="16">
-        <f>SUM(Q13:Q14)</f>
+      <c r="S15" s="15">
+        <f>SUM(S13:S14)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
+    <row r="16" spans="1:19">
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="19"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="K10:O10"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
     <mergeCell ref="P10:P11"/>
     <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="O10:O11"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:AA16"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" style="2" customWidth="1"/>
-    <col min="3" max="11" width="11" style="2" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="14" style="2" customWidth="1"/>
-    <col min="14" max="20" width="11" style="2" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="11" style="2" customWidth="1"/>
-    <col min="23" max="23" width="12.5703125" style="2" customWidth="1"/>
-    <col min="24" max="24" width="17.7109375" style="2" customWidth="1"/>
-    <col min="25" max="25" width="23.140625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="23.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" style="2" customWidth="1"/>
+    <col min="5" max="13" width="11" style="2" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="14" style="2" customWidth="1"/>
+    <col min="16" max="22" width="11" style="2" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="11" style="2" customWidth="1"/>
+    <col min="25" max="25" width="12.5703125" style="2" customWidth="1"/>
+    <col min="26" max="26" width="17.7109375" style="2" customWidth="1"/>
+    <col min="27" max="27" width="23.140625" style="2" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:27">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1097,12 +1247,14 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
-    </row>
-    <row r="2" spans="1:25">
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1120,12 +1272,14 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
-    </row>
-    <row r="3" spans="1:25">
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+    </row>
+    <row r="3" spans="1:27">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1143,372 +1297,398 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
-    </row>
-    <row r="5" spans="1:25">
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:27">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:27">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="1" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:27" s="1" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A10" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="C10" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="E10" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="F10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="19" t="s">
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="P10" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="19" t="s">
+      <c r="X10" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y10" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z10" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA10" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" s="1" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="V10" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="W10" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="X10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y10" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" s="1" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="I11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J11" s="4" t="s">
+      <c r="M11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="M11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="N11" s="4" t="s">
+      <c r="P11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="O11" s="20"/>
-      <c r="P11" s="4" t="s">
+      <c r="Q11" s="27"/>
+      <c r="R11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="4" t="s">
+      <c r="S11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="T11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="S11" s="4" t="s">
+      <c r="U11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="V11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="U11" s="20"/>
-      <c r="V11" s="20"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="20"/>
-    </row>
-    <row r="12" spans="1:25">
+      <c r="W11" s="27"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="23"/>
+      <c r="Z11" s="27"/>
+      <c r="AA11" s="27"/>
+    </row>
+    <row r="12" spans="1:27">
       <c r="A12" s="5">
         <v>1</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5">
         <v>2</v>
       </c>
-      <c r="C12" s="5">
+      <c r="E12" s="5">
         <v>3</v>
       </c>
-      <c r="D12" s="5">
+      <c r="F12" s="5">
         <v>4</v>
       </c>
-      <c r="E12" s="5">
+      <c r="G12" s="5">
         <v>5</v>
       </c>
-      <c r="F12" s="5">
+      <c r="H12" s="5">
         <v>6</v>
       </c>
-      <c r="G12" s="5">
+      <c r="I12" s="5">
         <v>7</v>
       </c>
-      <c r="H12" s="5">
+      <c r="J12" s="5">
         <v>8</v>
       </c>
-      <c r="I12" s="5">
+      <c r="K12" s="5">
         <v>9</v>
       </c>
-      <c r="J12" s="5">
+      <c r="L12" s="5">
         <v>10</v>
       </c>
-      <c r="K12" s="5">
+      <c r="M12" s="5">
         <v>11</v>
       </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5">
+      <c r="N12" s="5"/>
+      <c r="O12" s="5">
         <v>13</v>
       </c>
-      <c r="N12" s="5">
+      <c r="P12" s="5">
         <v>14</v>
       </c>
-      <c r="O12" s="5">
+      <c r="Q12" s="5">
         <v>15</v>
       </c>
-      <c r="P12" s="5">
+      <c r="R12" s="5">
         <v>16</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="S12" s="5">
         <v>17</v>
       </c>
-      <c r="R12" s="5">
+      <c r="T12" s="5">
         <v>18</v>
       </c>
-      <c r="S12" s="5">
+      <c r="U12" s="5">
         <v>19</v>
       </c>
-      <c r="T12" s="5">
+      <c r="V12" s="5">
         <v>20</v>
       </c>
-      <c r="U12" s="5">
+      <c r="W12" s="5">
         <v>21</v>
       </c>
-      <c r="V12" s="5">
+      <c r="X12" s="5">
         <v>22</v>
       </c>
-      <c r="W12" s="5">
+      <c r="Y12" s="5">
         <v>23</v>
       </c>
-      <c r="X12" s="5">
+      <c r="Z12" s="5">
         <v>24</v>
       </c>
-      <c r="Y12" s="5">
+      <c r="AA12" s="5">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
-      <c r="A13" s="6">
-        <v>1</v>
-      </c>
-      <c r="B13" s="7" t="s">
+    <row r="13" spans="1:27">
+      <c r="A13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="8" t="s">
+      <c r="G13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="I13" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="J13" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="K13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="L13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="M13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="N13" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="O13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="M13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N13" s="8" t="s">
+      <c r="R13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O13" s="12" t="s">
+      <c r="S13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="U13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="V13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="W13" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="P13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="R13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="S13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="T13" s="8" t="s">
+      <c r="X13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="U13" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="V13" s="8" t="s">
+      <c r="Y13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="W13" s="6" t="s">
+      <c r="Z13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="X13" s="8" t="s">
+      <c r="AA13" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="Y13" s="8" t="s">
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="9"/>
-    </row>
-    <row r="15" spans="1:25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y15" s="16">
-        <f>SUM(Y13:Y14)</f>
+      <c r="AA15" s="15">
+        <f>SUM(AA13:AA14)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
+    <row r="16" spans="1:27">
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="V10:V11"/>
+  <mergeCells count="13">
+    <mergeCell ref="F10:P10"/>
+    <mergeCell ref="R10:V10"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="W10:W11"/>
     <mergeCell ref="X10:X11"/>
     <mergeCell ref="Y10:Y11"/>
-    <mergeCell ref="D10:N10"/>
-    <mergeCell ref="P10:T10"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="Z10:Z11"/>
+    <mergeCell ref="AA10:AA11"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>